<commit_message>
added changes to the model
</commit_message>
<xml_diff>
--- a/forex_prediction_results.xlsx
+++ b/forex_prediction_results.xlsx
@@ -481,7 +481,7 @@
         <v>141.6</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -509,7 +509,7 @@
         <v>141.58</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>140.26</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>141.56</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -901,7 +901,7 @@
         <v>141.62</v>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
@@ -1069,7 +1069,7 @@
         <v>142.88</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
@@ -1083,7 +1083,7 @@
         <v>142.88</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>142.6</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="n">
         <v>1</v>
@@ -1153,7 +1153,7 @@
         <v>142.84</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
@@ -1251,7 +1251,7 @@
         <v>143.68</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
@@ -1265,7 +1265,7 @@
         <v>143.68</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
@@ -1349,7 +1349,7 @@
         <v>144.37</v>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
         <v>0</v>
@@ -1461,7 +1461,7 @@
         <v>142.54</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
@@ -1475,7 +1475,7 @@
         <v>142.54</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" t="n">
         <v>1</v>
@@ -1643,7 +1643,7 @@
         <v>144.02</v>
       </c>
       <c r="C86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
@@ -1699,7 +1699,7 @@
         <v>143.97</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90" t="n">
         <v>0</v>

</xml_diff>